<commit_message>
第 8 次commit About 更新 excel 文件
</commit_message>
<xml_diff>
--- a/汇总.xlsx
+++ b/汇总.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98A01FD-08B1-435E-AA3B-CD3833DDB072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9051F371-1E93-4D98-896B-51027B6CDE27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
   <si>
     <t>火狐</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,21 @@
   <si>
     <t>谷歌chrome</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浏览器正常运行代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -145,6 +160,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -427,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -441,6 +462,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -508,7 +532,61 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
第 10 次commit About 更新 excel 文件
</commit_message>
<xml_diff>
--- a/汇总.xlsx
+++ b/汇总.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9051F371-1E93-4D98-896B-51027B6CDE27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790720EC-B966-4D7D-A768-AEC2345C3A18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>火狐</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,14 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>测试03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -148,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +174,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -579,8 +590,60 @@
       </c>
       <c r="C14" s="6"/>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>

</xml_diff>

<commit_message>
第 12 次commit About 更新 excel 文件
</commit_message>
<xml_diff>
--- a/汇总.xlsx
+++ b/汇总.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790720EC-B966-4D7D-A768-AEC2345C3A18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0ED819-E518-47FD-984C-03FFDBA8606C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>火狐</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,10 @@
   </si>
   <si>
     <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试04</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -459,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -637,18 +641,70 @@
       </c>
       <c r="C21" s="6"/>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>